<commit_message>
Dodalem wiecej pomiarów do recenzji
</commit_message>
<xml_diff>
--- a/algorytmy sortujące + recenzja/sortowania recenzja.xlsx
+++ b/algorytmy sortujące + recenzja/sortowania recenzja.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\przemo79a\Informatyka\SCI_INF\algorytmy sortujące + recenzja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1AD289-0D41-4B1C-81D6-A8C281C0B8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187CBC7C-788F-4B34-9767-53E149B30F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16284" yWindow="-1536" windowWidth="23256" windowHeight="12576" xr2:uid="{9C65DEA7-4800-4277-A1C5-827F890F31C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9C65DEA7-4800-4277-A1C5-827F890F31C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="114">
   <si>
     <t>Bubble sort</t>
   </si>
@@ -144,8 +144,224 @@
     <t>Ilość wartości:</t>
   </si>
   <si>
+    <t>10 milionów</t>
+  </si>
+  <si>
+    <t>1 milion</t>
+  </si>
+  <si>
+    <t>std:: sort</t>
+  </si>
+  <si>
+    <t>Quick Sort</t>
+  </si>
+  <si>
+    <t>4.51119</t>
+  </si>
+  <si>
+    <t>5.04612</t>
+  </si>
+  <si>
+    <t>11.009</t>
+  </si>
+  <si>
+    <t>0.449368</t>
+  </si>
+  <si>
+    <t>0.535016</t>
+  </si>
+  <si>
+    <t>0.460777</t>
+  </si>
+  <si>
+    <t>Próba nr 1</t>
+  </si>
+  <si>
+    <t>Próba nr 2</t>
+  </si>
+  <si>
+    <t>Próba nr 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0032109   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0058956   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0003087   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0002574   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.34496   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.298828   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.549173   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0040528   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0036309   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.10198   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.02113   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.77636   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0110898   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0101202   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">36.5172   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.02447   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.1405   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0251552   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0214213   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">82.4463   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.9245   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">32.9324   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0360986   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0312375  </t>
+  </si>
+  <si>
+    <t>0.0143759</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0143925   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0032949   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0059396   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0003184   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0003038   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.36098   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.297916   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.56094   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0045936   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0037434   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.52772   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.87983   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0112564   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0105842   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">34.1087   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.50341   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.9424   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0248914   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0211132   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">77.0259   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.9189   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">31.3833   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0378789   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0357559   </t>
+  </si>
+  <si>
+    <t>0.0002254</t>
+  </si>
+  <si>
+    <t>0.0031144</t>
+  </si>
+  <si>
+    <t>0.0032068</t>
+  </si>
+  <si>
+    <t>0.0002941</t>
+  </si>
+  <si>
+    <t>0.0088576</t>
+  </si>
+  <si>
+    <t>0.0090959</t>
+  </si>
+  <si>
+    <t>0.0185276</t>
+  </si>
+  <si>
+    <t>0.0186097</t>
+  </si>
+  <si>
+    <t>0.02928</t>
+  </si>
+  <si>
+    <t>0.0290124</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Jak widać na wykresie, bubble sort jest algorytmem, który najdłużej radził sobie z sortowaniem. Zaraz po nim, z również nie najlepszymi wynikami znalazły się sortowania przez wybór oraz przez wstawianie. Przechodzenie przez każdą wartość po kolei nie jest dobrym pomysłem. Najszybsze okazały się być sortowanie z biblioteki std:: oraz sortowania rekurencyjne quick i merge, których na wykresach nawet nie widać, ponieważ z tym, nad czym co bubble sort pracował ponad minutę, one poradziły sobie w mniej niż pół sekundy. Są one porównywalnie szbkie. Dzielą one zbiory na mniejsze wartości i wywołują samych siebie, co wpływa korzystnie na czas oczekiwania. Dla lepszego zobrazowania warto dodać, że Merge Sort (Sortowania przez scalanie) z </t>
+      <t xml:space="preserve">Jak widać na wykresie, bubble sort jest algorytmem, który najdłużej radził sobie z sortowaniem. Zaraz po nim, z również nie najlepszymi wynikami znalazły się sortowania przez wybór oraz przez wstawianie. Przechodzenie przez każdą wartość po kolei nie jest dobrym pomysłem. Najszybsze okazały się być sortowanie z biblioteki std:: oraz sortowania rekurencyjne quick i merge, których na wykresach nawet nie widać, ponieważ z tym, nad czym co bubble sort pracował ponad minutę, one poradziły sobie w mniej niż pół sekundy. Algorytmy, których nie widać na pierwszym wykresie są porównywalnie szybkie. Dzielą one zbiory na mniejsze wartości i wywołują same siebie, co wpływa korzystnie na czas oczekiwania. Dla lepszego zobrazowania warto dodać, że Merge Sort (Sortowania przez scalanie) z </t>
     </r>
     <r>
       <rPr>
@@ -168,45 +384,30 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>wartości poradził sobie w 5 sekund, a std:: sort w 4,5 sekndy, gdzie bubble sortowi poukładanie 100tys. wartości zajmuje kilka minut.</t>
+      <t>wartości poradził sobie w 5 sekund, a std:: sort w 4,5 sekndy, gdzie bubble sortowi poukładanie 100tys. wartości zajmuje kilka minut. Stworzyłem osobny wyrkes dla sortowań, które okazały się być szybsze, aby mogły pokazać, na co je stać.</t>
     </r>
   </si>
   <si>
-    <t>10 milionów</t>
-  </si>
-  <si>
-    <t>1 milion</t>
-  </si>
-  <si>
-    <t>std:: sort</t>
-  </si>
-  <si>
-    <t>Quick Sort</t>
-  </si>
-  <si>
-    <t>4.51119</t>
-  </si>
-  <si>
-    <t>5.04612</t>
-  </si>
-  <si>
-    <t>11.009</t>
-  </si>
-  <si>
-    <t>0.449368</t>
-  </si>
-  <si>
-    <t>0.535016</t>
-  </si>
-  <si>
-    <t>0.460777</t>
+    <t>20 milionów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35.8821 </t>
+  </si>
+  <si>
+    <t>10.3205</t>
+  </si>
+  <si>
+    <t>10.8807</t>
+  </si>
+  <si>
+    <t>WYKRES UŚREDNIONYCH WARTOŚCI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +419,30 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -260,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -283,17 +508,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -316,23 +583,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1089</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>176349</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>35293</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>12676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>316916</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>184242</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>90709</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>174549</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Obraz 11">
+        <xdr:cNvPr id="14" name="Obraz 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A4A81C8-84CE-4BA4-8CDB-875176D95DA2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E879B37-B679-4EC7-964E-63505DAA7D98}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -354,8 +621,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5011239" y="4176849"/>
-          <a:ext cx="4792577" cy="3265443"/>
+          <a:off x="7696114" y="203176"/>
+          <a:ext cx="4953988" cy="3400373"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -366,23 +633,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>11950</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>526677</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>55418</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>4352</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>829236</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>118627</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Obraz 13">
+        <xdr:cNvPr id="3" name="Obraz 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E879B37-B679-4EC7-964E-63505DAA7D98}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62E2AF30-2D79-4ECA-A85E-C3519375A10F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -404,8 +671,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7661564" y="399877"/>
-          <a:ext cx="4932218" cy="3483748"/>
+          <a:off x="526677" y="6970059"/>
+          <a:ext cx="5322794" cy="3670892"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -714,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB986613-7C26-468C-8BC6-12FB4C1F57D7}">
-  <dimension ref="A2:G24"/>
+  <dimension ref="A1:Y61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,15 +999,36 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="J1" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
@@ -762,8 +1050,9 @@
       <c r="G3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1000</v>
       </c>
@@ -785,8 +1074,9 @@
       <c r="G4" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="23"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>10000</v>
       </c>
@@ -808,8 +1098,9 @@
       <c r="G5" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="23"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>25000</v>
       </c>
@@ -831,8 +1122,9 @@
       <c r="G6" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>50000</v>
       </c>
@@ -854,8 +1146,9 @@
       <c r="G7" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>75000</v>
       </c>
@@ -877,144 +1170,687 @@
       <c r="G8" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+    </row>
+    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>25000</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>50000</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>75000</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="I19" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+    </row>
+    <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>1000</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>25000</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="17">
+        <v>1079719</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>50000</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+    </row>
+    <row r="26" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>75000</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="E29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="8" t="s">
+      <c r="D31" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="11"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="11"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="11"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="11"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+    </row>
+    <row r="51" spans="20:25" x14ac:dyDescent="0.25">
+      <c r="T51" s="9"/>
+      <c r="U51" s="9"/>
+      <c r="V51" s="9"/>
+      <c r="W51" s="9"/>
+      <c r="X51" s="9"/>
+      <c r="Y51" s="9"/>
+    </row>
+    <row r="52" spans="20:25" x14ac:dyDescent="0.25">
+      <c r="T52" s="9"/>
+      <c r="U52" s="9"/>
+      <c r="V52" s="9"/>
+      <c r="W52" s="9"/>
+      <c r="X52" s="9"/>
+      <c r="Y52" s="9"/>
+    </row>
+    <row r="53" spans="20:25" x14ac:dyDescent="0.25">
+      <c r="T53" s="9"/>
+      <c r="U53" s="9"/>
+      <c r="V53" s="9"/>
+      <c r="W53" s="9"/>
+      <c r="X53" s="9"/>
+      <c r="Y53" s="9"/>
+    </row>
+    <row r="54" spans="20:25" x14ac:dyDescent="0.25">
+      <c r="T54" s="9"/>
+      <c r="U54" s="9"/>
+      <c r="V54" s="9"/>
+      <c r="W54" s="9"/>
+      <c r="X54" s="9"/>
+      <c r="Y54" s="9"/>
+    </row>
+    <row r="55" spans="20:25" x14ac:dyDescent="0.25">
+      <c r="T55" s="9"/>
+      <c r="U55" s="9"/>
+      <c r="V55" s="9"/>
+      <c r="W55" s="9"/>
+      <c r="X55" s="9"/>
+      <c r="Y55" s="9"/>
+    </row>
+    <row r="56" spans="20:25" x14ac:dyDescent="0.25">
+      <c r="T56" s="9"/>
+      <c r="U56" s="9"/>
+      <c r="V56" s="9"/>
+      <c r="W56" s="9"/>
+      <c r="X56" s="9"/>
+      <c r="Y56" s="9"/>
+    </row>
+    <row r="57" spans="20:25" x14ac:dyDescent="0.25">
+      <c r="T57" s="9"/>
+      <c r="U57" s="9"/>
+      <c r="V57" s="9"/>
+      <c r="W57" s="9"/>
+      <c r="X57" s="9"/>
+      <c r="Y57" s="9"/>
+    </row>
+    <row r="58" spans="20:25" x14ac:dyDescent="0.25">
+      <c r="T58" s="9"/>
+      <c r="U58" s="9"/>
+      <c r="V58" s="9"/>
+      <c r="W58" s="9"/>
+      <c r="X58" s="9"/>
+      <c r="Y58" s="9"/>
+    </row>
+    <row r="59" spans="20:25" x14ac:dyDescent="0.25">
+      <c r="T59" s="9"/>
+      <c r="U59" s="9"/>
+      <c r="V59" s="9"/>
+      <c r="W59" s="9"/>
+      <c r="X59" s="9"/>
+      <c r="Y59" s="9"/>
+    </row>
+    <row r="60" spans="20:25" x14ac:dyDescent="0.25">
+      <c r="T60" s="9"/>
+      <c r="U60" s="9"/>
+      <c r="V60" s="9"/>
+      <c r="W60" s="9"/>
+      <c r="X60" s="9"/>
+      <c r="Y60" s="9"/>
+    </row>
+    <row r="61" spans="20:25" x14ac:dyDescent="0.25">
+      <c r="T61" s="9"/>
+      <c r="U61" s="9"/>
+      <c r="V61" s="9"/>
+      <c r="W61" s="9"/>
+      <c r="X61" s="9"/>
+      <c r="Y61" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B10:G20"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="I19:P32"/>
+    <mergeCell ref="J1:O1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>